<commit_message>
feat: refactor modul 1 zapiska
</commit_message>
<xml_diff>
--- a/zapiska/sem7zapiska/Dlya_kursacha.xlsx
+++ b/zapiska/sem7zapiska/Dlya_kursacha.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Для курсача\Пример курсача\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\diplom\zapiska\sem7zapiska\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02936D11-4073-4C83-AFB4-46965C122F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4605" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20616" yWindow="4608" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,12 +222,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -271,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,12 +290,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -564,24 +576,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:I58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -604,7 +616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>1</v>
       </c>
@@ -620,7 +632,7 @@
       </c>
       <c r="G3" s="5">
         <f>10/(F3-E15)</f>
-        <v>2.6118326118326118</v>
+        <v>2.5531914893617018</v>
       </c>
       <c r="H3" s="5">
         <f>(1/(F3-1))+(1/(F3-2))+(1/(F3-3))+(1/(F3-4))+(1/(F3-5))+(1/(F3-6))+(1/(F3-7))+(1/(F3-8))+(1/(F3-9))+(1/(F3-10))</f>
@@ -628,53 +640,53 @@
       </c>
       <c r="I3" s="5">
         <f>H3-G3</f>
-        <v>0.31713564213564194</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+        <v>0.37577676460655196</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" ref="E4:E12" si="0">PRODUCT(C4,D4)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4" s="8">
         <v>12</v>
       </c>
       <c r="G4" s="5">
         <f>10/(F4-E15)</f>
-        <v>2.0709382151029749</v>
+        <v>2.0338983050847457</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:H12" si="1">(1/(F4-1))+(1/(F4-2))+(1/(F4-3))+(1/(F4-4))+(1/(F4-5))+(1/(F4-6))+(1/(F4-7))+(1/(F4-8))+(1/(F4-9))+(1/(F4-10))</f>
         <v>2.0198773448773446</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" ref="I4:I12" si="2">H4-G4</f>
-        <v>-5.1060870225630328E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I4:I11" si="2">H4-G4</f>
+        <v>-1.4020960207401068E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F5" s="8">
         <v>13</v>
       </c>
       <c r="G5" s="5">
         <f>10/(F5-E15)</f>
-        <v>1.7156398104265402</v>
+        <v>1.6901408450704225</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="1"/>
@@ -682,26 +694,26 @@
       </c>
       <c r="I5" s="5">
         <f t="shared" si="2"/>
-        <v>-0.11242913221586215</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-8.6930166859744418E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F6" s="8">
         <v>14</v>
       </c>
       <c r="G6" s="5">
         <f>10/(F6-E15)</f>
-        <v>1.464401294498382</v>
+        <v>1.4457831325301205</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
@@ -709,10 +721,10 @@
       </c>
       <c r="I6" s="5">
         <f t="shared" si="2"/>
-        <v>-0.11760087269796027</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-9.8982710729698775E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>5</v>
       </c>
@@ -728,7 +740,7 @@
       </c>
       <c r="G7" s="5">
         <f>10/(F7-E15)</f>
-        <v>1.2773465067043048</v>
+        <v>1.263157894736842</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="1"/>
@@ -736,26 +748,26 @@
       </c>
       <c r="I7" s="5">
         <f t="shared" si="2"/>
-        <v>-0.10911751347531173</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-9.492890150784894E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F8" s="8">
         <v>16</v>
       </c>
       <c r="G8" s="5">
         <f>10/(F8-E15)</f>
-        <v>1.1326658322903629</v>
+        <v>1.1214953271028036</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="1"/>
@@ -763,53 +775,53 @@
       </c>
       <c r="I8" s="5">
         <f t="shared" si="2"/>
-        <v>-9.7770172394703092E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-8.6599667207143849E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F9" s="8">
         <v>17</v>
       </c>
       <c r="G9" s="5">
         <f>10/(F9-E15)</f>
-        <v>1.0174255199550308</v>
+        <v>1.0084033613445378</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>0.93072899322899305</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="2"/>
-        <v>-8.6696526726037781E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+        <f>H9-G9</f>
+        <v>-7.7674368115544734E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="F10" s="8">
         <v>18</v>
       </c>
       <c r="G10" s="5">
         <f>10/(F10-E15)</f>
-        <v>0.92346938775510201</v>
+        <v>0.9160305343511449</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="1"/>
@@ -817,26 +829,26 @@
       </c>
       <c r="I10" s="5">
         <f t="shared" si="2"/>
-        <v>-7.6774007971487035E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-6.9335154567529922E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>9</v>
       </c>
       <c r="D11" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="F11" s="8">
         <v>19</v>
       </c>
       <c r="G11" s="5">
         <f>10/(F11-E15)</f>
-        <v>0.84539934609995326</v>
+        <v>0.83916083916083906</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="1"/>
@@ -844,59 +856,59 @@
       </c>
       <c r="I11" s="5">
         <f t="shared" si="2"/>
-        <v>-6.8148410760782707E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+        <v>-6.1909903821668499E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="F12" s="8">
         <v>20</v>
       </c>
       <c r="G12" s="5">
         <f>10/(F12-E15)</f>
-        <v>0.77950043066322139</v>
+        <v>0.77419354838709675</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="1"/>
         <v>0.71877140317542787</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="2"/>
-        <v>-6.0729027487793519E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+        <f>H12-G12</f>
+        <v>-5.5422145211668883E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="5">
         <f>SUM(D3:D12)</f>
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="E13" s="5">
         <f>SUM(E3:E12)</f>
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="5">
         <f>E13/D13</f>
-        <v>7.1712707182320443</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+        <v>7.083333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>9</v>
       </c>
@@ -907,64 +919,64 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="5">
         <f>10/((E17*D13)-E13)</f>
-        <v>1.1441647597254004E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1.059322033898305E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="5">
         <f>E19*((E17-1)-9)</f>
-        <v>2.2883295194508008E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+        <v>2.1186440677966101E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="5">
         <f>POWER(2.71828182846,-E21)</f>
-        <v>0.97737654165677457</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" ht="18.75" x14ac:dyDescent="0.3">
+        <v>0.97903641533965058</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
       <c r="E29" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F29" s="1">
-        <v>0.9</v>
+        <v>0.11</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="1">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F30" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G30" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
       <c r="E31" s="1">
         <v>0</v>
       </c>
@@ -972,87 +984,87 @@
         <v>0.2</v>
       </c>
       <c r="G31" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
       <c r="E33" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>17</v>
       </c>
       <c r="E34" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="E35" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>18</v>
       </c>
       <c r="E37" s="5">
         <f>E33*E29+E34*E30+E35*E31</f>
-        <v>0.154</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.38400000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="5">
         <f>E33*F29+E34*F30+E35*F31</f>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>20</v>
       </c>
       <c r="E39" s="5">
         <f>E33*G29+E34*G30+E35*G31</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>21</v>
       </c>
       <c r="E41" s="5">
         <f>E37*E29+E38*E30+E39*E31</f>
-        <v>8.678000000000001E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.19192000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>22</v>
       </c>
       <c r="E42" s="5">
         <f>E37*F29+E38*F30+E39*F31</f>
-        <v>0.35460000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+        <v>0.40514</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>23</v>
       </c>
       <c r="E43" s="5">
         <f>E37*G29+E38*G30+E39*G31</f>
-        <v>0.75599999999999989</v>
-      </c>
-    </row>
-    <row r="46" spans="4:7" ht="18.75" x14ac:dyDescent="0.3">
+        <v>1.3307</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D48" t="s">
         <v>25</v>
       </c>
@@ -1066,20 +1078,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D49" s="6">
-        <v>6.5000000000000002E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="E49" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F49" s="5">
         <f>MIN(D49,E49)</f>
-        <v>6.5000000000000002E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="G49" s="5">
         <f>(F49*(E49-1))/$I$49</f>
-        <v>1.2999999999999999E-3</v>
+        <v>1.98E-3</v>
       </c>
       <c r="H49" t="s">
         <v>28</v>
@@ -1087,21 +1099,22 @@
       <c r="I49" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="50" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="10"/>
+    </row>
+    <row r="50" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D50" s="7">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="E50" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F50" s="5">
         <f t="shared" ref="F50:F55" si="3">MIN(D50,E50)</f>
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="G50" s="5">
         <f t="shared" ref="G50:G55" si="4">(F50*(E50-1))/$I$49</f>
-        <v>2.4649999999999998E-2</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="H50" t="s">
         <v>29</v>
@@ -1109,26 +1122,27 @@
       <c r="I50" s="1">
         <v>130</v>
       </c>
-    </row>
-    <row r="51" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="9"/>
+    </row>
+    <row r="51" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D51" s="7">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E51" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F51" s="5">
         <f t="shared" si="3"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G51" s="5">
         <f t="shared" si="4"/>
-        <v>1.4000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.8000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D52" s="7">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E52" s="7">
         <v>0</v>
@@ -1142,61 +1156,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E53" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F53" s="5">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G53" s="5">
         <f t="shared" si="4"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.2000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D54" s="7">
-        <v>7.5800000000000006E-2</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="E54" s="7">
         <v>1</v>
       </c>
       <c r="F54" s="5">
         <f t="shared" si="3"/>
-        <v>7.5800000000000006E-2</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="G54" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E55" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F55" s="5">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G55" s="5">
         <f t="shared" si="4"/>
-        <v>1.5000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>30</v>
       </c>
       <c r="E58" s="5">
         <f>I50/I49+G49+G50+G51+G52+G53+G54+G55</f>
-        <v>0.68384999999999985</v>
+        <v>0.70028000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finish zapiska sem 7
</commit_message>
<xml_diff>
--- a/zapiska/sem7zapiska/Dlya_kursacha.xlsx
+++ b/zapiska/sem7zapiska/Dlya_kursacha.xlsx
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="C38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,13 +1091,13 @@
       </c>
       <c r="G49" s="5">
         <f>(F49*(E49-1))/$I$49</f>
-        <v>1.98E-3</v>
+        <v>2.0842105263157895E-3</v>
       </c>
       <c r="H49" t="s">
         <v>28</v>
       </c>
       <c r="I49" s="1">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J49" s="10"/>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="G50" s="5">
         <f t="shared" ref="G50:G55" si="4">(F50*(E50-1))/$I$49</f>
-        <v>2.8500000000000001E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="H50" t="s">
         <v>29</v>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="G51" s="5">
         <f t="shared" si="4"/>
-        <v>2.8000000000000004E-3</v>
+        <v>2.9473684210526317E-3</v>
       </c>
     </row>
     <row r="52" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G53" s="5">
         <f t="shared" si="4"/>
-        <v>1.2000000000000002E-2</v>
+        <v>1.2631578947368423E-2</v>
       </c>
     </row>
     <row r="54" spans="4:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="G55" s="5">
         <f t="shared" si="4"/>
-        <v>5.0000000000000001E-3</v>
+        <v>5.263157894736842E-3</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.3">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E58" s="5">
         <f>I50/I49+G49+G50+G51+G52+G53+G54+G55</f>
-        <v>0.70028000000000001</v>
+        <v>0.7371368421052632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>